<commit_message>
Update a_prime_leet predict_views, predict_utils, result_views, result_utils, templates, urls, admin_views, admin_utils, models, forms
</commit_message>
<xml_diff>
--- a/a_prime_leet/data/prime_leet_data.xlsx
+++ b/a_prime_leet/data/prime_leet_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_prime_leet\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA85E29-6F77-4C30-817F-A8F5E91DE9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA9BC2E-EB08-43EF-BB5F-A7A7C183E811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" tabRatio="624" activeTab="1" xr2:uid="{FA0813FA-CB0F-4B59-8071-35577C31DB12}"/>
+    <workbookView xWindow="-27570" yWindow="9270" windowWidth="19020" windowHeight="16200" tabRatio="624" activeTab="1" xr2:uid="{FA0813FA-CB0F-4B59-8071-35577C31DB12}"/>
   </bookViews>
   <sheets>
     <sheet name="Leet" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="19">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,12 @@
     <t>추리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>언어</t>
+  </si>
+  <si>
+    <t>추리</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy&quot;-&quot;m&quot;-&quot;d\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,12 +182,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -672,10 +672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C8602B-517C-41CF-ADE2-D30699ECAC44}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -699,7 +699,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" cm="1">
-        <f t="array" ref="A2:A71">_xlfn.SEQUENCE(COUNT(B:B))</f>
+        <f t="array" ref="A2:A106">_xlfn.SEQUENCE(COUNT(B:B))</f>
         <v>1</v>
       </c>
       <c r="B2">
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -763,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -814,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -916,7 +916,7 @@
         <v>13</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -933,7 +933,7 @@
         <v>14</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -950,7 +950,7 @@
         <v>15</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -967,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1001,7 +1001,7 @@
         <v>18</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1018,7 +1018,7 @@
         <v>19</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1052,7 +1052,7 @@
         <v>21</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
         <v>22</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>23</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1120,7 +1120,7 @@
         <v>25</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>27</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1188,7 +1188,7 @@
         <v>29</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1205,7 +1205,7 @@
         <v>30</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1307,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1341,7 +1341,7 @@
         <v>8</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1358,7 +1358,7 @@
         <v>9</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1375,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1392,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1409,7 +1409,7 @@
         <v>12</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1426,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1443,7 +1443,7 @@
         <v>14</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1460,7 +1460,7 @@
         <v>15</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1477,7 +1477,7 @@
         <v>16</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1494,7 +1494,7 @@
         <v>17</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1511,7 +1511,7 @@
         <v>18</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1528,7 +1528,7 @@
         <v>19</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1579,7 +1579,7 @@
         <v>22</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1596,7 +1596,7 @@
         <v>23</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1613,7 +1613,7 @@
         <v>24</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1630,7 +1630,7 @@
         <v>25</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>26</v>
       </c>
       <c r="E57">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1664,7 +1664,7 @@
         <v>27</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
         <v>29</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1715,7 +1715,7 @@
         <v>30</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
         <v>31</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1749,7 +1749,7 @@
         <v>32</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1766,7 +1766,7 @@
         <v>33</v>
       </c>
       <c r="E64">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="E65">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1800,7 +1800,7 @@
         <v>35</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1834,7 +1834,7 @@
         <v>37</v>
       </c>
       <c r="E68">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1868,7 +1868,7 @@
         <v>39</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1885,7 +1885,602 @@
         <v>40</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78">
+        <v>7</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79">
+        <v>8</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80">
+        <v>9</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84">
+        <v>13</v>
+      </c>
+      <c r="E84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85">
+        <v>14</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86">
+        <v>15</v>
+      </c>
+      <c r="E86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+      <c r="E90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92">
+        <v>6</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93">
+        <v>7</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94">
+        <v>8</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96">
+        <v>10</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97">
+        <v>11</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98">
+        <v>12</v>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99">
+        <v>13</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100">
+        <v>14</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101">
+        <v>15</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102">
+        <v>16</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103">
+        <v>17</v>
+      </c>
+      <c r="E103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104">
+        <v>18</v>
+      </c>
+      <c r="E104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105">
+        <v>19</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106">
+        <v>20</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>